<commit_message>
Projeto final do curso Python do IPEA (finalizado)
</commit_message>
<xml_diff>
--- a/BD2.xlsx
+++ b/BD2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HFBiBru\PycharmProjects\Projeto-SMTR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HFa\PycharmProjects\Curso-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A5969A-05DD-46B6-94A9-ACF3376382F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D441AE4B-F707-4A8C-98D5-F1374D822EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{562EA06A-641A-45B5-B845-CFBDBC377A56}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{562EA06A-641A-45B5-B845-CFBDBC377A56}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
   <si>
     <t>ano</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>mes</t>
+  </si>
+  <si>
+    <t>tarifa</t>
   </si>
 </sst>
 </file>
@@ -418,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F660E8-DD0E-4FD8-97FA-5BEF5FE98525}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +446,9 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -457,6 +463,9 @@
       <c r="D2" s="2">
         <v>83711736</v>
       </c>
+      <c r="E2" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -471,6 +480,9 @@
       <c r="D3" s="2">
         <v>79719855</v>
       </c>
+      <c r="E3" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -485,6 +497,9 @@
       <c r="D4" s="2">
         <v>94974852</v>
       </c>
+      <c r="E4" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -499,6 +514,9 @@
       <c r="D5" s="2">
         <v>86829791</v>
       </c>
+      <c r="E5" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -513,6 +531,9 @@
       <c r="D6" s="2">
         <v>91745084</v>
       </c>
+      <c r="E6" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -527,6 +548,9 @@
       <c r="D7" s="2">
         <v>91611987</v>
       </c>
+      <c r="E7" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -541,6 +565,9 @@
       <c r="D8" s="2">
         <v>95491389</v>
       </c>
+      <c r="E8" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -555,6 +582,9 @@
       <c r="D9" s="2">
         <v>93613585</v>
       </c>
+      <c r="E9" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -569,6 +599,9 @@
       <c r="D10" s="2">
         <v>91155075</v>
       </c>
+      <c r="E10" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -583,6 +616,9 @@
       <c r="D11" s="2">
         <v>94218456</v>
       </c>
+      <c r="E11" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -597,6 +633,9 @@
       <c r="D12" s="2">
         <v>89052423</v>
       </c>
+      <c r="E12" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -610,6 +649,9 @@
       </c>
       <c r="D13" s="2">
         <v>92353215</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.4</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -695,7 +737,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,6 +761,9 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -733,6 +778,9 @@
       <c r="D2" s="2">
         <v>81487228</v>
       </c>
+      <c r="E2" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -747,6 +795,9 @@
       <c r="D3" s="2">
         <v>82747640</v>
       </c>
+      <c r="E3" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -761,6 +812,9 @@
       <c r="D4" s="2">
         <v>91890990</v>
       </c>
+      <c r="E4" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -775,6 +829,9 @@
       <c r="D5" s="2">
         <v>88623233</v>
       </c>
+      <c r="E5" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -789,6 +846,9 @@
       <c r="D6" s="2">
         <v>89275434</v>
       </c>
+      <c r="E6" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -803,6 +863,9 @@
       <c r="D7" s="2">
         <v>89251103</v>
       </c>
+      <c r="E7" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -817,6 +880,9 @@
       <c r="D8" s="2">
         <v>89526673</v>
       </c>
+      <c r="E8" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -831,6 +897,9 @@
       <c r="D9" s="2">
         <v>89332665</v>
       </c>
+      <c r="E9" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -845,6 +914,9 @@
       <c r="D10" s="2">
         <v>89676594</v>
       </c>
+      <c r="E10" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -859,6 +931,9 @@
       <c r="D11" s="2">
         <v>87147501</v>
       </c>
+      <c r="E11" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -873,6 +948,9 @@
       <c r="D12" s="2">
         <v>82980084</v>
       </c>
+      <c r="E12" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -886,6 +964,9 @@
       </c>
       <c r="D13" s="2">
         <v>85538838</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.8</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -971,7 +1052,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,6 +1076,9 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -1009,6 +1093,9 @@
       <c r="D2" s="2">
         <v>79250242</v>
       </c>
+      <c r="E2" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1023,6 +1110,9 @@
       <c r="D3" s="2">
         <v>73924867</v>
       </c>
+      <c r="E3" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1037,6 +1127,9 @@
       <c r="D4" s="2">
         <v>85836636</v>
       </c>
+      <c r="E4" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -1051,6 +1144,9 @@
       <c r="D5" s="2">
         <v>76334307</v>
       </c>
+      <c r="E5" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1065,6 +1161,9 @@
       <c r="D6" s="2">
         <v>85118308</v>
       </c>
+      <c r="E6" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1079,6 +1178,9 @@
       <c r="D7" s="2">
         <v>79691741</v>
       </c>
+      <c r="E7" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1093,6 +1195,9 @@
       <c r="D8" s="2">
         <v>78456997</v>
       </c>
+      <c r="E8" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1107,6 +1212,9 @@
       <c r="D9" s="2">
         <v>81811068</v>
       </c>
+      <c r="E9" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1121,6 +1229,9 @@
       <c r="D10" s="2">
         <v>79590199</v>
       </c>
+      <c r="E10" s="1">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1135,6 +1246,9 @@
       <c r="D11" s="2">
         <v>78495622</v>
       </c>
+      <c r="E11" s="1">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1149,6 +1263,9 @@
       <c r="D12" s="2">
         <v>76222050</v>
       </c>
+      <c r="E12" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1162,6 +1279,9 @@
       </c>
       <c r="D13" s="2">
         <v>78296401</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.4</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1247,7 +1367,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,6 +1391,9 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -1285,6 +1408,9 @@
       <c r="D2" s="2">
         <v>75487575</v>
       </c>
+      <c r="E2" s="1">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1299,6 +1425,9 @@
       <c r="D3" s="2">
         <v>66862646</v>
       </c>
+      <c r="E3" s="1">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1313,6 +1442,9 @@
       <c r="D4" s="2">
         <v>80139580</v>
       </c>
+      <c r="E4" s="1">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -1327,6 +1459,9 @@
       <c r="D5" s="2">
         <v>72756102</v>
       </c>
+      <c r="E5" s="1">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1341,6 +1476,9 @@
       <c r="D6" s="2">
         <v>73887491</v>
       </c>
+      <c r="E6" s="1">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1355,6 +1493,9 @@
       <c r="D7" s="2">
         <v>71632649</v>
       </c>
+      <c r="E7" s="1">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1369,6 +1510,9 @@
       <c r="D8" s="2">
         <v>73149297</v>
       </c>
+      <c r="E8" s="1">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1383,6 +1527,9 @@
       <c r="D9" s="2">
         <v>78081523</v>
       </c>
+      <c r="E9" s="1">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1397,6 +1544,9 @@
       <c r="D10" s="2">
         <v>71066648</v>
       </c>
+      <c r="E10" s="1">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1411,6 +1561,9 @@
       <c r="D11" s="2">
         <v>75785980</v>
       </c>
+      <c r="E11" s="1">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1425,6 +1578,9 @@
       <c r="D12" s="2">
         <v>69533054</v>
       </c>
+      <c r="E12" s="1">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1438,6 +1594,9 @@
       </c>
       <c r="D13" s="2">
         <v>71592636</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.95</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1520,10 +1679,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AD3C7C-8985-474B-82C5-235BF8C52FCD}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,7 +1693,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1547,8 +1706,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2019</v>
       </c>
@@ -1561,8 +1723,11 @@
       <c r="D2" s="2">
         <v>69442637</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2019</v>
       </c>
@@ -1575,8 +1740,11 @@
       <c r="D3" s="2">
         <v>66258639</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2019</v>
       </c>
@@ -1589,8 +1757,11 @@
       <c r="D4" s="2">
         <v>65554340</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2019</v>
       </c>
@@ -1603,8 +1774,11 @@
       <c r="D5" s="2">
         <v>66361228</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2019</v>
       </c>
@@ -1617,8 +1791,11 @@
       <c r="D6" s="2">
         <v>71011306</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2019</v>
       </c>
@@ -1631,8 +1808,11 @@
       <c r="D7" s="2">
         <v>64361061</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2019</v>
       </c>
@@ -1645,8 +1825,11 @@
       <c r="D8" s="2">
         <v>68702419</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2019</v>
       </c>
@@ -1659,8 +1842,11 @@
       <c r="D9" s="2">
         <v>68955453</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2019</v>
       </c>
@@ -1673,8 +1859,11 @@
       <c r="D10" s="2">
         <v>66329549</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2019</v>
       </c>
@@ -1687,8 +1876,11 @@
       <c r="D11" s="2">
         <v>70096547</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2019</v>
       </c>
@@ -1701,8 +1893,11 @@
       <c r="D12" s="2">
         <v>62711950</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2019</v>
       </c>
@@ -1714,6 +1909,9 @@
       </c>
       <c r="D13" s="2">
         <v>63746756</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.05</v>
       </c>
     </row>
   </sheetData>
@@ -1724,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D1AB31-0E1F-46C7-8275-DB7A592D155A}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1936,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1751,8 +1949,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2020</v>
       </c>
@@ -1765,8 +1966,11 @@
       <c r="D2" s="2">
         <v>60626481</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2020</v>
       </c>
@@ -1779,8 +1983,11 @@
       <c r="D3" s="2">
         <v>56041114</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2020</v>
       </c>
@@ -1793,8 +2000,11 @@
       <c r="D4" s="2">
         <v>46125539</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2020</v>
       </c>
@@ -1807,8 +2017,11 @@
       <c r="D5" s="2">
         <v>21210698</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2020</v>
       </c>
@@ -1821,8 +2034,11 @@
       <c r="D6" s="2">
         <v>22787262</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2020</v>
       </c>
@@ -1835,8 +2051,11 @@
       <c r="D7" s="2">
         <v>27585269</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2020</v>
       </c>
@@ -1849,8 +2068,11 @@
       <c r="D8" s="2">
         <v>35456174</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2020</v>
       </c>
@@ -1863,8 +2085,11 @@
       <c r="D9" s="2">
         <v>38269289</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2020</v>
       </c>
@@ -1877,8 +2102,11 @@
       <c r="D10" s="2">
         <v>39223166</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2020</v>
       </c>
@@ -1891,8 +2119,11 @@
       <c r="D11" s="2">
         <v>41472062</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2020</v>
       </c>
@@ -1905,8 +2136,11 @@
       <c r="D12" s="2">
         <v>40717541</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2020</v>
       </c>
@@ -1918,6 +2152,9 @@
       </c>
       <c r="D13" s="2">
         <v>41805408</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.05</v>
       </c>
     </row>
   </sheetData>
@@ -1930,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC3674A-1C1B-434C-AD4D-24624C8055FD}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,6 +2194,9 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -1971,6 +2211,9 @@
       <c r="D2" s="2">
         <v>39802206</v>
       </c>
+      <c r="E2" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1985,6 +2228,9 @@
       <c r="D3" s="2">
         <v>37154126</v>
       </c>
+      <c r="E3" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1999,6 +2245,9 @@
       <c r="D4" s="2">
         <v>40788490</v>
       </c>
+      <c r="E4" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -2013,6 +2262,9 @@
       <c r="D5" s="2">
         <v>36709109</v>
       </c>
+      <c r="E5" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -2027,6 +2279,9 @@
       <c r="D6" s="2">
         <v>40110251</v>
       </c>
+      <c r="E6" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -2041,6 +2296,9 @@
       <c r="D7" s="2">
         <v>41417205</v>
       </c>
+      <c r="E7" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -2055,6 +2313,9 @@
       <c r="D8" s="2">
         <v>44604921</v>
       </c>
+      <c r="E8" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -2069,6 +2330,9 @@
       <c r="D9" s="2">
         <v>45529377</v>
       </c>
+      <c r="E9" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -2083,6 +2347,9 @@
       <c r="D10" s="2">
         <v>44979812</v>
       </c>
+      <c r="E10" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -2097,6 +2364,9 @@
       <c r="D11" s="2">
         <v>46506189</v>
       </c>
+      <c r="E11" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -2111,6 +2381,9 @@
       <c r="D12" s="2">
         <v>46316869</v>
       </c>
+      <c r="E12" s="1">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -2124,6 +2397,9 @@
       </c>
       <c r="D13" s="2">
         <v>48250521</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.05</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>